<commit_message>
KIBON-1662 KindId in Excel ausgeblendet hinzugefügt.
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/KinderMitZemisNummer.xlsx
+++ b/ebegu-server/src/main/resources/reporting/KinderMitZemisNummer.xlsx
@@ -8,21 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE7B855-0986-4BC3-B4C0-EEEF851618F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AD573B-12E2-4EFD-A92E-06A8BC976720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{1AEF1F9C-938D-450B-BF9F-74AAB8E05F65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{FDCBD70C-8A11-49D6-823B-8BF5A48C20E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="eingabeLastenausgleich">Data!$H$7</definedName>
-    <definedName name="korrektur">Data!#REF!</definedName>
-    <definedName name="kostenProHundertProzentPlatz">Data!$F$7</definedName>
-    <definedName name="selbstbehaltGemeinde">Data!$G$7</definedName>
-    <definedName name="totalBelegung">Data!$D$7</definedName>
-    <definedName name="totalGutscheine">Data!$E$7</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -42,7 +34,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>Kinder mit Zemis Nummer</t>
+  </si>
   <si>
     <t>Parameter</t>
   </si>
@@ -50,61 +45,64 @@
     <t>Jahr</t>
   </si>
   <si>
+    <t>Fall</t>
+  </si>
+  <si>
+    <t>Periode</t>
+  </si>
+  <si>
+    <t>Gemeinde</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Vorname</t>
+  </si>
+  <si>
+    <t>Geburtsdatum</t>
+  </si>
+  <si>
+    <t>ZEMIS Nummer</t>
+  </si>
+  <si>
+    <t>Kein Selbstbehalt für die Gemeinde</t>
+  </si>
+  <si>
+    <t>{fall}</t>
+  </si>
+  <si>
+    <t>{periode}</t>
+  </si>
+  <si>
+    <t>{gemeinde}</t>
+  </si>
+  <si>
+    <t>{name}</t>
+  </si>
+  <si>
+    <t>{vorname}</t>
+  </si>
+  <si>
+    <t>{geburtsdatum}</t>
+  </si>
+  <si>
+    <t>{zemisNummer}</t>
+  </si>
+  <si>
+    <t>{keinSelbstbehaltFuerGemeinde}</t>
+  </si>
+  <si>
+    <t>{repeatRow}</t>
+  </si>
+  <si>
     <t>{berechnungsjahr}</t>
   </si>
   <si>
-    <t>Gemeinde</t>
-  </si>
-  <si>
-    <t>{repeatRow}</t>
-  </si>
-  <si>
-    <t>{gemeinde}</t>
-  </si>
-  <si>
-    <t>Fall</t>
-  </si>
-  <si>
-    <t>{fall}</t>
-  </si>
-  <si>
-    <t>Periode</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Vorname</t>
-  </si>
-  <si>
-    <t>Geburtsdatum</t>
-  </si>
-  <si>
-    <t>ZEMIS Nummer</t>
-  </si>
-  <si>
-    <t>Kein Selbstbehalt für die Gemeinde</t>
-  </si>
-  <si>
-    <t>{periode}</t>
-  </si>
-  <si>
-    <t>{name}</t>
-  </si>
-  <si>
-    <t>{vorname}</t>
-  </si>
-  <si>
-    <t>{geburtsdatum}</t>
-  </si>
-  <si>
-    <t>{zemisNummer}</t>
-  </si>
-  <si>
-    <t>{keinSelbstbehaltFuerGemeinde}</t>
-  </si>
-  <si>
-    <t>Kinder mit Zemis Nummer</t>
+    <t>Kind ID</t>
+  </si>
+  <si>
+    <t>{kindId}</t>
   </si>
 </sst>
 </file>
@@ -114,13 +112,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;CHF&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,8 +121,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -145,7 +136,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -199,19 +191,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -235,16 +224,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color theme="5" tint="-0.499984740745262"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFF7C5A7"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF7C5A7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -552,104 +546,107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0BAB2BE-640F-45EA-ADC8-77B8E625E64E}">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A6B590-44C6-472F-AF4D-09A68C6B8FEE}">
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.75" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11" style="3"/>
-    <col min="4" max="4" width="15.25" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18" style="3" customWidth="1"/>
-    <col min="8" max="8" width="30.375" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="11" style="3"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="E6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="H6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="I6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="F7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="I7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="J7" t="s">
         <v>19</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H7">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>FALSE</formula>
+  <conditionalFormatting sqref="I1:I10 I13:I1048576">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>AND(NOT(ISBLANK(I1)),I1=FALSE)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
KIBON-1662 Kind Nummer statt ID in Excel
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/KinderMitZemisNummer.xlsx
+++ b/ebegu-server/src/main/resources/reporting/KinderMitZemisNummer.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu2\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AD573B-12E2-4EFD-A92E-06A8BC976720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C234A885-5363-440B-89A6-0081FE41375E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{FDCBD70C-8A11-49D6-823B-8BF5A48C20E7}"/>
   </bookViews>
@@ -99,10 +99,10 @@
     <t>{berechnungsjahr}</t>
   </si>
   <si>
-    <t>Kind ID</t>
-  </si>
-  <si>
     <t>{kindId}</t>
+  </si>
+  <si>
+    <t>Kind Nummer</t>
   </si>
 </sst>
 </file>
@@ -191,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -207,6 +207,11 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -555,7 +560,7 @@
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" style="11" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.28515625" customWidth="1"/>
     <col min="9" max="9" width="33.140625" bestFit="1" customWidth="1"/>
@@ -596,8 +601,8 @@
       <c r="E6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>21</v>
+      <c r="F6" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>8</v>
@@ -625,8 +630,8 @@
       <c r="E7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>22</v>
+      <c r="F7" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
KIBON-1663 Write correct value for keinSelbstbehaltFuerGemeinde in ZEMIS Excel
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/KinderMitZemisNummer.xlsx
+++ b/ebegu-server/src/main/resources/reporting/KinderMitZemisNummer.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu2\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C234A885-5363-440B-89A6-0081FE41375E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A905554C-358D-4902-9BF0-C79C6D6F9297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{FDCBD70C-8A11-49D6-823B-8BF5A48C20E7}"/>
   </bookViews>
@@ -216,7 +216,27 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7C5A7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -647,11 +667,11 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I1:I10 I13:I1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>AND(NOT(ISBLANK(I1)),I1=FALSE)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>